<commit_message>
Refactor investment tools CLI and data workflows
</commit_message>
<xml_diff>
--- a/perspective_shares.xlsx
+++ b/perspective_shares.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -750,6 +750,100 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PHOR</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ФосАгро</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>9978b56f-782a-4a80-a4b1-a48cbecfd194</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PHOR</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>RU000A0JRKT8</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>BBG004S689R0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>TQBR</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>share</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>5a3d1efd-f8a0-478e-a10e-bb7f990f9c87</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HEAD</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Хэдхантер</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3fe80143-1313-42eb-9884-5d68b39e265e</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>HEAD</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>RU000A107662</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>TCS20A107662</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>TQBR</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>share</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>911552ef-a892-4b33-9df1-c0d6c4a2307d</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>